<commit_message>
Renamed "Price" to "Cost" in our data
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -1258,7 +1258,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* \-??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* \-??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="General"/>
     <numFmt numFmtId="168" formatCode="#,##0;[RED]\-#,##0"/>
   </numFmts>
   <fonts count="12">
@@ -1530,7 +1530,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1591,7 +1591,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1639,27 +1639,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="6" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="6" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="7" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="7" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1675,7 +1675,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="7" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="7" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1683,11 +1683,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1703,7 +1703,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1711,15 +1711,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="10" fillId="3" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1751,7 +1751,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="5" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="5" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1836,10 +1836,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2116,7 +2112,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="22.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="60" width="84.94"/>
@@ -2802,7 +2798,7 @@
       <selection pane="topLeft" activeCell="G52" activeCellId="0" sqref="G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="21.36"/>
@@ -3449,11 +3445,11 @@
   </sheetPr>
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
   </cols>
@@ -3502,7 +3498,7 @@
         <v>9</v>
       </c>
       <c r="O1" s="20" t="s">
-        <v>17</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3515,34 +3511,34 @@
       <c r="E2" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="F2" s="77" t="n">
+      <c r="F2" s="13" t="n">
         <v>6</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="H2" s="77" t="n">
+      <c r="H2" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="I2" s="77" t="n">
+      <c r="I2" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="J2" s="77" t="n">
+      <c r="J2" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="K2" s="77" t="n">
+      <c r="K2" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="L2" s="77" t="n">
+      <c r="L2" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="M2" s="77" t="n">
+      <c r="M2" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="N2" s="77" t="n">
+      <c r="N2" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="O2" s="78" t="n">
+      <c r="O2" s="77" t="n">
         <v>85</v>
       </c>
     </row>
@@ -3556,7 +3552,7 @@
       <c r="E3" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="F3" s="77" t="n">
+      <c r="F3" s="13" t="n">
         <v>6</v>
       </c>
       <c r="G3" s="0" t="n">
@@ -3565,25 +3561,25 @@
       <c r="H3" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="I3" s="77" t="n">
+      <c r="I3" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="J3" s="77" t="n">
+      <c r="J3" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="K3" s="77" t="n">
+      <c r="K3" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="L3" s="77" t="n">
+      <c r="L3" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="M3" s="77" t="n">
+      <c r="M3" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="N3" s="77" t="n">
+      <c r="N3" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="O3" s="78" t="n">
+      <c r="O3" s="77" t="n">
         <v>90</v>
       </c>
     </row>
@@ -3594,34 +3590,34 @@
       <c r="E4" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="F4" s="77" t="n">
+      <c r="F4" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="G4" s="77" t="n">
+      <c r="G4" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H4" s="77" t="n">
+      <c r="H4" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="I4" s="77" t="n">
+      <c r="I4" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="J4" s="77" t="n">
+      <c r="J4" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="K4" s="77" t="n">
+      <c r="K4" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="L4" s="77" t="n">
+      <c r="L4" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="M4" s="77" t="n">
+      <c r="M4" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="N4" s="77" t="n">
+      <c r="N4" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="O4" s="77" t="n">
+      <c r="O4" s="13" t="n">
         <v>70</v>
       </c>
     </row>
@@ -3632,34 +3628,34 @@
       <c r="E5" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="F5" s="77" t="n">
+      <c r="F5" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="G5" s="77" t="n">
+      <c r="G5" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H5" s="77" t="n">
+      <c r="H5" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="I5" s="77" t="n">
+      <c r="I5" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="J5" s="77" t="n">
+      <c r="J5" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="K5" s="77" t="n">
+      <c r="K5" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="L5" s="77" t="n">
+      <c r="L5" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="M5" s="77" t="n">
+      <c r="M5" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="N5" s="77" t="n">
+      <c r="N5" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="O5" s="77" t="n">
+      <c r="O5" s="13" t="n">
         <v>75</v>
       </c>
     </row>
@@ -3670,34 +3666,34 @@
       <c r="E6" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="F6" s="77" t="n">
+      <c r="F6" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="G6" s="77" t="n">
+      <c r="G6" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H6" s="77" t="n">
+      <c r="H6" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="I6" s="77" t="n">
+      <c r="I6" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="J6" s="77" t="n">
+      <c r="J6" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="K6" s="77" t="n">
+      <c r="K6" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="L6" s="77" t="n">
+      <c r="L6" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="M6" s="77" t="n">
+      <c r="M6" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="N6" s="77" t="n">
+      <c r="N6" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="O6" s="77" t="n">
+      <c r="O6" s="13" t="n">
         <v>85</v>
       </c>
     </row>
@@ -3708,34 +3704,34 @@
       <c r="E7" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="F7" s="77" t="n">
+      <c r="F7" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="G7" s="77" t="n">
+      <c r="G7" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H7" s="77" t="n">
+      <c r="H7" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="I7" s="77" t="n">
+      <c r="I7" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="J7" s="77" t="n">
+      <c r="J7" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="K7" s="77" t="n">
+      <c r="K7" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="L7" s="77" t="n">
+      <c r="L7" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="M7" s="77" t="n">
+      <c r="M7" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="N7" s="77" t="n">
+      <c r="N7" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="O7" s="77" t="n">
+      <c r="O7" s="13" t="n">
         <v>110</v>
       </c>
     </row>
@@ -3746,34 +3742,34 @@
       <c r="E8" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="F8" s="77" t="n">
+      <c r="F8" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="G8" s="77" t="n">
+      <c r="G8" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H8" s="77" t="n">
+      <c r="H8" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="I8" s="77" t="n">
+      <c r="I8" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="J8" s="77" t="n">
+      <c r="J8" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="K8" s="77" t="n">
+      <c r="K8" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="L8" s="77" t="n">
+      <c r="L8" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="M8" s="77" t="n">
+      <c r="M8" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="N8" s="77" t="n">
+      <c r="N8" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="O8" s="77" t="n">
+      <c r="O8" s="13" t="n">
         <v>215</v>
       </c>
     </row>
@@ -3784,34 +3780,34 @@
       <c r="E9" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="F9" s="77" t="n">
+      <c r="F9" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="G9" s="77" t="n">
+      <c r="G9" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="H9" s="77" t="n">
+      <c r="H9" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="I9" s="77" t="n">
+      <c r="I9" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="J9" s="77" t="n">
+      <c r="J9" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="K9" s="77" t="n">
+      <c r="K9" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="L9" s="77" t="n">
+      <c r="L9" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="M9" s="77" t="n">
+      <c r="M9" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="N9" s="77" t="n">
+      <c r="N9" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="O9" s="77" t="n">
+      <c r="O9" s="13" t="n">
         <v>215</v>
       </c>
     </row>
@@ -3833,11 +3829,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B73" activeCellId="0" sqref="B73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="36.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.67"/>
@@ -7124,11 +7120,11 @@
   </sheetPr>
   <dimension ref="A1:CB74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BD1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="BF27" activeCellId="0" sqref="BF27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="20.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.4"/>
@@ -13176,7 +13172,7 @@
       <selection pane="topLeft" activeCell="M68" activeCellId="0" sqref="M68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
@@ -13300,11 +13296,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.67"/>
@@ -13364,7 +13360,7 @@
         <v>9</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>17</v>
+        <v>144</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
@@ -15094,10 +15090,10 @@
   <dimension ref="A1:AE63"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R24" activeCellId="0" sqref="R24"/>
+      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="28.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.65"/>
@@ -17767,7 +17763,7 @@
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="21.48"/>
   </cols>
@@ -17866,7 +17862,7 @@
   </sheetPr>
   <dimension ref="A1:AMD49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N53" activeCellId="0" sqref="N53"/>
     </sheetView>
   </sheetViews>
@@ -17882,7 +17878,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="20.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="50.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="18.79"/>
@@ -64109,7 +64105,7 @@
       <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
   </cols>

</xml_diff>

<commit_message>
Nippon Leves missing attributes fix
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\245439\dv\warhammer-list-builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F2D119-D4C4-40BA-846A-A795DF5BB3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A14CBA-FD3C-4A85-A69F-29B70AC7B63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13890" yWindow="-16365" windowWidth="29040" windowHeight="15840" tabRatio="840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fantasy_Baseline_Stats" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2797" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2796" uniqueCount="451">
   <si>
     <t>M</t>
   </si>
@@ -7832,8 +7832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CL89"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="AE8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="12.75" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
@@ -7917,6 +7917,7 @@
     <col min="81" max="81" width="24" bestFit="1" customWidth="1"/>
     <col min="82" max="82" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="85" max="85" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9621,45 +9622,530 @@
       <c r="CL12" s="34"/>
     </row>
     <row r="13" spans="1:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L13" s="1"/>
-      <c r="M13" t="s">
-        <v>140</v>
-      </c>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
+      <c r="J13" s="42" t="str">
+        <f>CONCATENATE(J$1,"_","Secondary_Weaponry")</f>
+        <v>Empire_State_Troop_Secondary_Weaponry</v>
+      </c>
+      <c r="K13" s="42" t="str">
+        <f t="shared" ref="K13:BY20" si="4">CONCATENATE(K$1,"_","Secondary_Weaponry")</f>
+        <v>Empire_State_Troop_Skirmisher_Secondary_Weaponry</v>
+      </c>
+      <c r="L13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Reiksguard_Secondary_Weaponry</v>
+      </c>
+      <c r="M13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Empire_Captain_Secondary_Weaponry</v>
+      </c>
+      <c r="N13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_Engineer_Secondary_Weaponry</v>
+      </c>
+      <c r="O13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Greatsword_Secondary_Weaponry</v>
+      </c>
+      <c r="P13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Halfling_Secondary_Weaponry</v>
+      </c>
+      <c r="Q13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Mounted_Empire_Captain_Secondary_Weaponry</v>
+      </c>
+      <c r="R13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Mounted_Reiksguard_Secondary_Weaponry</v>
+      </c>
+      <c r="S13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Witch_Hunter_Secondary_Weaponry</v>
+      </c>
+      <c r="T13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Swordmaster_Secondary_Weaponry</v>
+      </c>
+      <c r="U13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>White_Lion_Secondary_Weaponry</v>
+      </c>
+      <c r="V13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Phoenix_Guard_Secondary_Weaponry</v>
+      </c>
+      <c r="W13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Archer_Secondary_Weaponry</v>
+      </c>
+      <c r="X13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Noble_Secondary_Weaponry</v>
+      </c>
+      <c r="Y13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Mounted_Noble_Secondary_Weaponry</v>
+      </c>
+      <c r="Z13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Silver_Helm_Secondary_Weaponry</v>
+      </c>
+      <c r="AA13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Shadow_Warrior_Secondary_Weaponry</v>
+      </c>
+      <c r="AB13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Sea_Guard_Secondary_Weaponry</v>
+      </c>
+      <c r="AC13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Orc_Boy_Secondary_Weaponry</v>
+      </c>
+      <c r="AD13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Big_Un_Secondary_Weaponry</v>
+      </c>
+      <c r="AE13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Black_Orc_Secondary_Weaponry</v>
+      </c>
+      <c r="AF13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Savage_orc_Secondary_Weaponry</v>
+      </c>
+      <c r="AG13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Savage_Orc_Big_Un_Secondary_Weaponry</v>
+      </c>
+      <c r="AH13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Orc_Big_Boss_Secondary_Weaponry</v>
+      </c>
+      <c r="AI13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Arrer_Boy_Secondary_Weaponry</v>
+      </c>
+      <c r="AJ13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Night_Goblin_Secondary_Weaponry</v>
+      </c>
+      <c r="AK13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Night_Goblin_Big_Boss_Secondary_Weaponry</v>
+      </c>
+      <c r="AL13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Mounted_Night_Goblin_Big_Boss_Secondary_Weaponry</v>
+      </c>
+      <c r="AM13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Troll_Secondary_Weaponry</v>
+      </c>
+      <c r="AN13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Peasant_Secondary_Weaponry</v>
+      </c>
+      <c r="AO13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Bowman_Secondary_Weaponry</v>
+      </c>
+      <c r="AP13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Brettonian_Foot_Knight_Secondary_Weaponry</v>
+      </c>
+      <c r="AQ13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Mounted_Brettonian_Knight_Secondary_Weaponry</v>
+      </c>
+      <c r="AR13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Brettonian_Knight_Secondary_Weaponry</v>
+      </c>
+      <c r="AS13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Duke_Secondary_Weaponry</v>
+      </c>
+      <c r="AT13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Skavenslave_Secondary_Weaponry</v>
+      </c>
+      <c r="AU13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Clan_Rat_Secondary_Weaponry</v>
+      </c>
+      <c r="AV13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Gutter_Runner_Secondary_Weaponry</v>
+      </c>
+      <c r="AW13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Storm_Vermin_Secondary_Weaponry</v>
+      </c>
+      <c r="AX13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Rat_Ogre_Secondary_Weaponry</v>
+      </c>
+      <c r="AY13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Claw_Leader_Secondary_Weaponry</v>
+      </c>
+      <c r="AZ13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Mounted_Claw_Leader_Secondary_Weaponry</v>
+      </c>
+      <c r="BA13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Dwarf_Warrior_Secondary_Weaponry</v>
+      </c>
+      <c r="BB13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Slayer_Secondary_Weaponry</v>
+      </c>
+      <c r="BC13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Ironbreaker_Secondary_Weaponry</v>
+      </c>
+      <c r="BD13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Hammerer_Secondary_Weaponry</v>
+      </c>
+      <c r="BE13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Dwarf_Captain_Secondary_Weaponry</v>
+      </c>
+      <c r="BF13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Mounted_Warrior_of_Chaos_Secondary_Weaponry</v>
+      </c>
+      <c r="BG13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Warrior_of_Chaos_Secondary_Weaponry</v>
+      </c>
+      <c r="BH13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Marauder_Secondary_Weaponry</v>
+      </c>
+      <c r="BI13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Mounted_Exalted_Champion_Secondary_Weaponry</v>
+      </c>
+      <c r="BJ13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Exalted_Champion_Secondary_Weaponry</v>
+      </c>
+      <c r="BK13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Dark_Elf_Warrior_Secondary_Weaponry</v>
+      </c>
+      <c r="BL13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Dreadknight_Secondary_Weaponry</v>
+      </c>
+      <c r="BM13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Witch_Elf_Secondary_Weaponry</v>
+      </c>
+      <c r="BN13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Dark_Elf_Corsair_Secondary_Weaponry</v>
+      </c>
+      <c r="BO13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Executioner_Secondary_Weaponry</v>
+      </c>
+      <c r="BP13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Shade_Secondary_Weaponry</v>
+      </c>
+      <c r="BQ13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Mounted_Dark_Elf_Master_Secondary_Weaponry</v>
+      </c>
+      <c r="BR13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Dark_Elf_Master_Secondary_Weaponry</v>
+      </c>
+      <c r="BS13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Cathayan_Captain_Secondary_Weaponry</v>
+      </c>
+      <c r="BT13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Mounted_Cathayan_Captain_Secondary_Weaponry</v>
+      </c>
+      <c r="BU13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Dragon_Cavalry_Secondary_Weaponry</v>
+      </c>
+      <c r="BV13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Imperial_Infantry_Secondary_Weaponry</v>
+      </c>
+      <c r="BW13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Levy-Infantry_Secondary_Weaponry</v>
+      </c>
+      <c r="BX13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Dragonblade_Secondary_Weaponry</v>
+      </c>
+      <c r="BY13" s="42" t="str">
+        <f t="shared" si="4"/>
+        <v>Imperial_Guard_Secondary_Weaponry</v>
+      </c>
+      <c r="BZ13" s="42" t="str">
+        <f t="shared" ref="BZ13:CE20" si="5">CONCATENATE(BZ$1,"_","Secondary_Weaponry")</f>
+        <v>Temple_Dog_Secondary_Weaponry</v>
+      </c>
+      <c r="CA13" s="42" t="str">
+        <f t="shared" si="5"/>
+        <v>Hatamoto_Secondary_Weaponry</v>
+      </c>
+      <c r="CB13" s="42" t="str">
+        <f t="shared" si="5"/>
+        <v>Mounted_Hatamoto_Secondary_Weaponry</v>
+      </c>
+      <c r="CC13" s="42" t="str">
+        <f t="shared" si="5"/>
+        <v>Samurai_Secondary_Weaponry</v>
+      </c>
+      <c r="CD13" s="42" t="str">
+        <f t="shared" si="5"/>
+        <v>Mounted_Samurai_Secondary_Weaponry</v>
+      </c>
+      <c r="CE13" s="42" t="str">
+        <f t="shared" si="5"/>
+        <v>Ashiguru_Secondary_Weaponry</v>
+      </c>
+      <c r="CF13" s="42" t="str">
+        <f>CONCATENATE(CF$1,"_","Secondary_Weaponry")</f>
+        <v>Nipponese_Leves_Secondary_Weaponry</v>
+      </c>
       <c r="CG13" s="35" t="str">
-        <f t="shared" ref="CG13:CL13" si="4">CONCATENATE(CG$1,"_","Secondary_Weaponry")</f>
+        <f t="shared" ref="CG13:CL13" si="6">CONCATENATE(CG$1,"_","Secondary_Weaponry")</f>
         <v>Jarl_Secondary_Weaponry</v>
       </c>
       <c r="CH13" s="35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Hersir_Secondary_Weaponry</v>
       </c>
       <c r="CI13" s="35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Hirdmen_Secondary_Weaponry</v>
       </c>
       <c r="CJ13" s="35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Shield_Maiden_Secondary_Weaponry</v>
       </c>
       <c r="CK13" s="35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Berserker_Secondary_Weaponry</v>
       </c>
       <c r="CL13" s="35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Bondi_Secondary_Weaponry</v>
       </c>
     </row>
     <row r="14" spans="1:90" ht="15" x14ac:dyDescent="0.25">
-      <c r="L14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="U14" s="1"/>
+      <c r="J14" t="s">
+        <v>170</v>
+      </c>
+      <c r="K14" t="s">
+        <v>170</v>
+      </c>
+      <c r="L14" t="s">
+        <v>168</v>
+      </c>
+      <c r="M14" t="s">
+        <v>170</v>
+      </c>
+      <c r="N14" t="s">
+        <v>168</v>
+      </c>
+      <c r="O14" s="43"/>
+      <c r="P14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>168</v>
+      </c>
+      <c r="R14" t="s">
+        <v>168</v>
+      </c>
+      <c r="S14" t="s">
+        <v>129</v>
+      </c>
+      <c r="T14" s="29"/>
+      <c r="U14" s="29"/>
+      <c r="X14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>327</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AV14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AX14" t="s">
+        <v>133</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>168</v>
+      </c>
+      <c r="AZ14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BA14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BB14" t="s">
+        <v>129</v>
+      </c>
+      <c r="BC14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BD14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BE14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BF14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BG14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BH14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BI14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BJ14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BK14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BL14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BM14" t="s">
+        <v>327</v>
+      </c>
+      <c r="BN14" t="s">
+        <v>129</v>
+      </c>
+      <c r="BP14" t="s">
+        <v>327</v>
+      </c>
+      <c r="BQ14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BR14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BS14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BT14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BU14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BV14" t="s">
+        <v>168</v>
+      </c>
+      <c r="BW14" t="s">
+        <v>168</v>
+      </c>
+      <c r="CA14" t="s">
+        <v>327</v>
+      </c>
+      <c r="CB14" t="s">
+        <v>327</v>
+      </c>
+      <c r="CC14" t="s">
+        <v>169</v>
+      </c>
+      <c r="CD14" t="s">
+        <v>327</v>
+      </c>
+      <c r="CE14" t="s">
+        <v>169</v>
+      </c>
+      <c r="CF14" t="s">
+        <v>327</v>
+      </c>
       <c r="CG14" s="36" t="s">
         <v>168</v>
       </c>
@@ -9680,13 +10166,177 @@
       </c>
     </row>
     <row r="15" spans="1:90" ht="15" x14ac:dyDescent="0.25">
-      <c r="L15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="U15" s="1"/>
+      <c r="J15" t="s">
+        <v>168</v>
+      </c>
+      <c r="K15" t="s">
+        <v>168</v>
+      </c>
+      <c r="L15" t="s">
+        <v>129</v>
+      </c>
+      <c r="M15" t="s">
+        <v>168</v>
+      </c>
+      <c r="N15" t="s">
+        <v>327</v>
+      </c>
+      <c r="P15" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>129</v>
+      </c>
+      <c r="R15" t="s">
+        <v>129</v>
+      </c>
+      <c r="S15" t="s">
+        <v>327</v>
+      </c>
+      <c r="X15" t="s">
+        <v>327</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>327</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>327</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AO15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AS15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>327</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>327</v>
+      </c>
+      <c r="AV15" t="s">
+        <v>327</v>
+      </c>
+      <c r="AW15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>129</v>
+      </c>
+      <c r="AZ15" t="s">
+        <v>129</v>
+      </c>
+      <c r="BA15" t="s">
+        <v>129</v>
+      </c>
+      <c r="BB15" t="s">
+        <v>327</v>
+      </c>
+      <c r="BC15" t="s">
+        <v>129</v>
+      </c>
+      <c r="BE15" t="s">
+        <v>129</v>
+      </c>
+      <c r="BF15" t="s">
+        <v>129</v>
+      </c>
+      <c r="BG15" t="s">
+        <v>129</v>
+      </c>
+      <c r="BH15" t="s">
+        <v>129</v>
+      </c>
+      <c r="BI15" t="s">
+        <v>129</v>
+      </c>
+      <c r="BJ15" t="s">
+        <v>129</v>
+      </c>
+      <c r="BK15" t="s">
+        <v>327</v>
+      </c>
+      <c r="BL15" t="s">
+        <v>327</v>
+      </c>
+      <c r="BN15" t="s">
+        <v>327</v>
+      </c>
+      <c r="BP15" t="s">
+        <v>136</v>
+      </c>
+      <c r="BQ15" t="s">
+        <v>327</v>
+      </c>
+      <c r="BR15" t="s">
+        <v>327</v>
+      </c>
+      <c r="BS15" t="s">
+        <v>129</v>
+      </c>
+      <c r="BT15" t="s">
+        <v>129</v>
+      </c>
+      <c r="BU15" t="s">
+        <v>129</v>
+      </c>
+      <c r="BV15" t="s">
+        <v>129</v>
+      </c>
+      <c r="BW15" t="s">
+        <v>129</v>
+      </c>
+      <c r="CC15" t="s">
+        <v>327</v>
+      </c>
+      <c r="CE15" t="s">
+        <v>327</v>
+      </c>
       <c r="CG15" s="34" t="s">
         <v>231</v>
       </c>
@@ -9707,13 +10357,165 @@
       </c>
     </row>
     <row r="16" spans="1:90" ht="15" x14ac:dyDescent="0.25">
-      <c r="L16" s="1"/>
-      <c r="O16" s="1"/>
+      <c r="J16" t="s">
+        <v>128</v>
+      </c>
+      <c r="K16" t="s">
+        <v>129</v>
+      </c>
+      <c r="L16" t="s">
+        <v>327</v>
+      </c>
+      <c r="M16" t="s">
+        <v>129</v>
+      </c>
+      <c r="N16" t="s">
+        <v>128</v>
+      </c>
       <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
+      <c r="Q16" t="s">
+        <v>327</v>
+      </c>
+      <c r="R16" t="s">
+        <v>327</v>
+      </c>
+      <c r="S16" t="s">
+        <v>128</v>
+      </c>
+      <c r="T16" s="29"/>
+      <c r="U16" s="29"/>
+      <c r="X16" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>128</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AO16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AQ16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AS16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AU16" t="s">
+        <v>128</v>
+      </c>
+      <c r="AV16" t="s">
+        <v>128</v>
+      </c>
+      <c r="AW16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AY16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AZ16" t="s">
+        <v>327</v>
+      </c>
+      <c r="BA16" t="s">
+        <v>327</v>
+      </c>
+      <c r="BB16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BC16" t="s">
+        <v>327</v>
+      </c>
+      <c r="BE16" t="s">
+        <v>327</v>
+      </c>
+      <c r="BF16" t="s">
+        <v>327</v>
+      </c>
+      <c r="BG16" t="s">
+        <v>327</v>
+      </c>
+      <c r="BH16" t="s">
+        <v>327</v>
+      </c>
+      <c r="BI16" t="s">
+        <v>327</v>
+      </c>
+      <c r="BJ16" t="s">
+        <v>327</v>
+      </c>
+      <c r="BK16" t="s">
+        <v>128</v>
+      </c>
+      <c r="BL16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BN16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BP16" t="s">
+        <v>128</v>
+      </c>
+      <c r="BQ16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BR16" t="s">
+        <v>136</v>
+      </c>
+      <c r="BS16" t="s">
+        <v>327</v>
+      </c>
+      <c r="BT16" t="s">
+        <v>327</v>
+      </c>
+      <c r="BU16" t="s">
+        <v>327</v>
+      </c>
+      <c r="BV16" t="s">
+        <v>327</v>
+      </c>
+      <c r="BW16" t="s">
+        <v>327</v>
+      </c>
       <c r="CG16" s="34" t="s">
         <v>327</v>
       </c>
@@ -9734,16 +10536,129 @@
       </c>
     </row>
     <row r="17" spans="10:90" ht="15" x14ac:dyDescent="0.25">
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="O17" s="1"/>
+      <c r="J17" t="s">
+        <v>129</v>
+      </c>
+      <c r="K17" t="s">
+        <v>327</v>
+      </c>
+      <c r="L17" t="s">
+        <v>136</v>
+      </c>
+      <c r="M17" t="s">
+        <v>327</v>
+      </c>
       <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
+      <c r="Q17" t="s">
+        <v>136</v>
+      </c>
+      <c r="R17" t="s">
+        <v>136</v>
+      </c>
       <c r="T17" s="29"/>
       <c r="U17" s="29"/>
+      <c r="AC17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>128</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AW17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AY17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AZ17" t="s">
+        <v>136</v>
+      </c>
+      <c r="BA17" t="s">
+        <v>136</v>
+      </c>
+      <c r="BC17" t="s">
+        <v>136</v>
+      </c>
+      <c r="BE17" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF17" t="s">
+        <v>136</v>
+      </c>
+      <c r="BG17" t="s">
+        <v>136</v>
+      </c>
+      <c r="BH17" t="s">
+        <v>136</v>
+      </c>
+      <c r="BI17" t="s">
+        <v>136</v>
+      </c>
+      <c r="BJ17" t="s">
+        <v>136</v>
+      </c>
+      <c r="BL17" t="s">
+        <v>128</v>
+      </c>
+      <c r="BN17" t="s">
+        <v>128</v>
+      </c>
+      <c r="BQ17" t="s">
+        <v>128</v>
+      </c>
+      <c r="BR17" t="s">
+        <v>128</v>
+      </c>
+      <c r="BS17" t="s">
+        <v>136</v>
+      </c>
+      <c r="BT17" t="s">
+        <v>136</v>
+      </c>
+      <c r="BU17" t="s">
+        <v>136</v>
+      </c>
+      <c r="BV17" t="s">
+        <v>136</v>
+      </c>
+      <c r="BW17" t="s">
+        <v>128</v>
+      </c>
       <c r="CG17" s="34" t="s">
         <v>128</v>
       </c>
@@ -9762,16 +10677,95 @@
       <c r="CL17" s="34"/>
     </row>
     <row r="18" spans="10:90" ht="15" x14ac:dyDescent="0.25">
-      <c r="J18" s="1"/>
+      <c r="J18" t="s">
+        <v>136</v>
+      </c>
       <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="O18" s="1"/>
+      <c r="L18" t="s">
+        <v>128</v>
+      </c>
+      <c r="M18" t="s">
+        <v>136</v>
+      </c>
       <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
+      <c r="Q18" t="s">
+        <v>128</v>
+      </c>
+      <c r="R18" t="s">
+        <v>128</v>
+      </c>
       <c r="S18" s="1"/>
       <c r="T18" s="29"/>
       <c r="U18" s="29"/>
+      <c r="AC18" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>128</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>128</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>128</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>128</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>128</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>128</v>
+      </c>
+      <c r="AQ18" t="s">
+        <v>128</v>
+      </c>
+      <c r="AR18" t="s">
+        <v>128</v>
+      </c>
+      <c r="AS18" t="s">
+        <v>128</v>
+      </c>
+      <c r="AW18" t="s">
+        <v>128</v>
+      </c>
+      <c r="AY18" t="s">
+        <v>128</v>
+      </c>
+      <c r="AZ18" t="s">
+        <v>128</v>
+      </c>
+      <c r="BE18" t="s">
+        <v>128</v>
+      </c>
+      <c r="BF18" t="s">
+        <v>128</v>
+      </c>
+      <c r="BG18" t="s">
+        <v>128</v>
+      </c>
+      <c r="BH18" t="s">
+        <v>128</v>
+      </c>
+      <c r="BI18" t="s">
+        <v>128</v>
+      </c>
+      <c r="BJ18" t="s">
+        <v>128</v>
+      </c>
+      <c r="BS18" t="s">
+        <v>128</v>
+      </c>
+      <c r="BT18" t="s">
+        <v>128</v>
+      </c>
+      <c r="BU18" t="s">
+        <v>128</v>
+      </c>
+      <c r="BV18" t="s">
+        <v>128</v>
+      </c>
       <c r="CG18" s="34"/>
       <c r="CH18" s="34"/>
       <c r="CI18" s="34"/>
@@ -9780,10 +10774,14 @@
       <c r="CL18" s="34"/>
     </row>
     <row r="19" spans="10:90" ht="15" x14ac:dyDescent="0.25">
-      <c r="J19" s="1"/>
+      <c r="J19" t="s">
+        <v>327</v>
+      </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="O19" s="1"/>
+      <c r="M19" t="s">
+        <v>128</v>
+      </c>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -9797,307 +10795,16 @@
       <c r="CK19" s="34"/>
       <c r="CL19" s="34"/>
     </row>
-    <row r="20" spans="10:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J20" s="42" t="str">
-        <f>CONCATENATE(J$1,"_","Secondary_Weaponry")</f>
-        <v>Empire_State_Troop_Secondary_Weaponry</v>
-      </c>
-      <c r="K20" s="42" t="str">
-        <f t="shared" ref="K20:BY20" si="5">CONCATENATE(K$1,"_","Secondary_Weaponry")</f>
-        <v>Empire_State_Troop_Skirmisher_Secondary_Weaponry</v>
-      </c>
-      <c r="L20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Reiksguard_Secondary_Weaponry</v>
-      </c>
-      <c r="M20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Empire_Captain_Secondary_Weaponry</v>
-      </c>
-      <c r="N20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Master_Engineer_Secondary_Weaponry</v>
-      </c>
-      <c r="O20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Greatsword_Secondary_Weaponry</v>
-      </c>
-      <c r="P20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Halfling_Secondary_Weaponry</v>
-      </c>
-      <c r="Q20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Mounted_Empire_Captain_Secondary_Weaponry</v>
-      </c>
-      <c r="R20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Mounted_Reiksguard_Secondary_Weaponry</v>
-      </c>
-      <c r="S20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Witch_Hunter_Secondary_Weaponry</v>
-      </c>
-      <c r="T20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Swordmaster_Secondary_Weaponry</v>
-      </c>
-      <c r="U20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>White_Lion_Secondary_Weaponry</v>
-      </c>
-      <c r="V20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Phoenix_Guard_Secondary_Weaponry</v>
-      </c>
-      <c r="W20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Archer_Secondary_Weaponry</v>
-      </c>
-      <c r="X20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Noble_Secondary_Weaponry</v>
-      </c>
-      <c r="Y20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Mounted_Noble_Secondary_Weaponry</v>
-      </c>
-      <c r="Z20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Silver_Helm_Secondary_Weaponry</v>
-      </c>
-      <c r="AA20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Shadow_Warrior_Secondary_Weaponry</v>
-      </c>
-      <c r="AB20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Sea_Guard_Secondary_Weaponry</v>
-      </c>
-      <c r="AC20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Orc_Boy_Secondary_Weaponry</v>
-      </c>
-      <c r="AD20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Big_Un_Secondary_Weaponry</v>
-      </c>
-      <c r="AE20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Black_Orc_Secondary_Weaponry</v>
-      </c>
-      <c r="AF20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Savage_orc_Secondary_Weaponry</v>
-      </c>
-      <c r="AG20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Savage_Orc_Big_Un_Secondary_Weaponry</v>
-      </c>
-      <c r="AH20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Orc_Big_Boss_Secondary_Weaponry</v>
-      </c>
-      <c r="AI20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Arrer_Boy_Secondary_Weaponry</v>
-      </c>
-      <c r="AJ20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Night_Goblin_Secondary_Weaponry</v>
-      </c>
-      <c r="AK20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Night_Goblin_Big_Boss_Secondary_Weaponry</v>
-      </c>
-      <c r="AL20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Mounted_Night_Goblin_Big_Boss_Secondary_Weaponry</v>
-      </c>
-      <c r="AM20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Troll_Secondary_Weaponry</v>
-      </c>
-      <c r="AN20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Peasant_Secondary_Weaponry</v>
-      </c>
-      <c r="AO20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Bowman_Secondary_Weaponry</v>
-      </c>
-      <c r="AP20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Brettonian_Foot_Knight_Secondary_Weaponry</v>
-      </c>
-      <c r="AQ20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Mounted_Brettonian_Knight_Secondary_Weaponry</v>
-      </c>
-      <c r="AR20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Brettonian_Knight_Secondary_Weaponry</v>
-      </c>
-      <c r="AS20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Duke_Secondary_Weaponry</v>
-      </c>
-      <c r="AT20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Skavenslave_Secondary_Weaponry</v>
-      </c>
-      <c r="AU20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Clan_Rat_Secondary_Weaponry</v>
-      </c>
-      <c r="AV20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Gutter_Runner_Secondary_Weaponry</v>
-      </c>
-      <c r="AW20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Storm_Vermin_Secondary_Weaponry</v>
-      </c>
-      <c r="AX20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Rat_Ogre_Secondary_Weaponry</v>
-      </c>
-      <c r="AY20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Claw_Leader_Secondary_Weaponry</v>
-      </c>
-      <c r="AZ20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Mounted_Claw_Leader_Secondary_Weaponry</v>
-      </c>
-      <c r="BA20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Dwarf_Warrior_Secondary_Weaponry</v>
-      </c>
-      <c r="BB20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Slayer_Secondary_Weaponry</v>
-      </c>
-      <c r="BC20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Ironbreaker_Secondary_Weaponry</v>
-      </c>
-      <c r="BD20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Hammerer_Secondary_Weaponry</v>
-      </c>
-      <c r="BE20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Dwarf_Captain_Secondary_Weaponry</v>
-      </c>
-      <c r="BF20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Mounted_Warrior_of_Chaos_Secondary_Weaponry</v>
-      </c>
-      <c r="BG20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Warrior_of_Chaos_Secondary_Weaponry</v>
-      </c>
-      <c r="BH20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Marauder_Secondary_Weaponry</v>
-      </c>
-      <c r="BI20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Mounted_Exalted_Champion_Secondary_Weaponry</v>
-      </c>
-      <c r="BJ20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Exalted_Champion_Secondary_Weaponry</v>
-      </c>
-      <c r="BK20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Dark_Elf_Warrior_Secondary_Weaponry</v>
-      </c>
-      <c r="BL20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Dreadknight_Secondary_Weaponry</v>
-      </c>
-      <c r="BM20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Witch_Elf_Secondary_Weaponry</v>
-      </c>
-      <c r="BN20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Dark_Elf_Corsair_Secondary_Weaponry</v>
-      </c>
-      <c r="BO20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Executioner_Secondary_Weaponry</v>
-      </c>
-      <c r="BP20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Shade_Secondary_Weaponry</v>
-      </c>
-      <c r="BQ20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Mounted_Dark_Elf_Master_Secondary_Weaponry</v>
-      </c>
-      <c r="BR20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Dark_Elf_Master_Secondary_Weaponry</v>
-      </c>
-      <c r="BS20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Cathayan_Captain_Secondary_Weaponry</v>
-      </c>
-      <c r="BT20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Mounted_Cathayan_Captain_Secondary_Weaponry</v>
-      </c>
-      <c r="BU20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Dragon_Cavalry_Secondary_Weaponry</v>
-      </c>
-      <c r="BV20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Imperial_Infantry_Secondary_Weaponry</v>
-      </c>
-      <c r="BW20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Levy-Infantry_Secondary_Weaponry</v>
-      </c>
-      <c r="BX20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Dragonblade_Secondary_Weaponry</v>
-      </c>
-      <c r="BY20" s="42" t="str">
-        <f t="shared" si="5"/>
-        <v>Imperial_Guard_Secondary_Weaponry</v>
-      </c>
-      <c r="BZ20" s="42" t="str">
-        <f t="shared" ref="BZ20:CE20" si="6">CONCATENATE(BZ$1,"_","Secondary_Weaponry")</f>
-        <v>Temple_Dog_Secondary_Weaponry</v>
-      </c>
-      <c r="CA20" s="42" t="str">
-        <f t="shared" si="6"/>
-        <v>Hatamoto_Secondary_Weaponry</v>
-      </c>
-      <c r="CB20" s="42" t="str">
-        <f t="shared" si="6"/>
-        <v>Mounted_Hatamoto_Secondary_Weaponry</v>
-      </c>
-      <c r="CC20" s="42" t="str">
-        <f t="shared" si="6"/>
-        <v>Samurai_Secondary_Weaponry</v>
-      </c>
-      <c r="CD20" s="42" t="str">
-        <f t="shared" si="6"/>
-        <v>Mounted_Samurai_Secondary_Weaponry</v>
-      </c>
-      <c r="CE20" s="42" t="str">
-        <f t="shared" si="6"/>
-        <v>Ashiguru_Secondary_Weaponry</v>
-      </c>
-      <c r="CF20" s="42" t="str">
-        <f>CONCATENATE(CF$1,"_","Secondary_Weaponry")</f>
-        <v>Nipponese_Leves_Secondary_Weaponry</v>
-      </c>
+    <row r="20" spans="10:90" ht="15" x14ac:dyDescent="0.25">
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="29"/>
+      <c r="U20" s="29"/>
       <c r="CG20" s="34"/>
       <c r="CH20" s="34"/>
       <c r="CI20" s="34"/>
@@ -10106,204 +10813,6 @@
       <c r="CL20" s="34"/>
     </row>
     <row r="21" spans="10:90" ht="15" x14ac:dyDescent="0.25">
-      <c r="J21" t="s">
-        <v>170</v>
-      </c>
-      <c r="K21" t="s">
-        <v>170</v>
-      </c>
-      <c r="L21" t="s">
-        <v>168</v>
-      </c>
-      <c r="M21" t="s">
-        <v>170</v>
-      </c>
-      <c r="N21" t="s">
-        <v>168</v>
-      </c>
-      <c r="O21" s="43"/>
-      <c r="P21" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>168</v>
-      </c>
-      <c r="R21" t="s">
-        <v>168</v>
-      </c>
-      <c r="S21" t="s">
-        <v>129</v>
-      </c>
-      <c r="T21" s="29"/>
-      <c r="U21" s="29"/>
-      <c r="X21" t="s">
-        <v>168</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>168</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>327</v>
-      </c>
-      <c r="AB21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AC21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AD21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AE21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AF21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AG21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AH21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AI21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AJ21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AK21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AL21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AN21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AO21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AP21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AQ21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AR21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AS21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AT21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AU21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AV21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AW21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AX21" t="s">
-        <v>133</v>
-      </c>
-      <c r="AY21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AZ21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BA21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BB21" t="s">
-        <v>129</v>
-      </c>
-      <c r="BC21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BD21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BE21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BF21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BG21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BH21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BI21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BJ21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BK21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BL21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BM21" t="s">
-        <v>327</v>
-      </c>
-      <c r="BN21" t="s">
-        <v>129</v>
-      </c>
-      <c r="BP21" t="s">
-        <v>327</v>
-      </c>
-      <c r="BQ21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BR21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BS21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BT21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BU21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BV21" t="s">
-        <v>168</v>
-      </c>
-      <c r="BW21" t="s">
-        <v>168</v>
-      </c>
-      <c r="CA21" t="s">
-        <v>327</v>
-      </c>
-      <c r="CB21" t="s">
-        <v>327</v>
-      </c>
-      <c r="CC21" t="s">
-        <v>169</v>
-      </c>
-      <c r="CD21" t="s">
-        <v>327</v>
-      </c>
-      <c r="CE21" t="s">
-        <v>169</v>
-      </c>
-      <c r="CF21" t="s">
-        <v>327</v>
-      </c>
       <c r="CG21" s="34"/>
       <c r="CH21" s="34"/>
       <c r="CI21" s="34"/>
@@ -10312,177 +10821,6 @@
       <c r="CL21" s="34"/>
     </row>
     <row r="22" spans="10:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J22" t="s">
-        <v>168</v>
-      </c>
-      <c r="K22" t="s">
-        <v>168</v>
-      </c>
-      <c r="L22" t="s">
-        <v>129</v>
-      </c>
-      <c r="M22" t="s">
-        <v>168</v>
-      </c>
-      <c r="N22" t="s">
-        <v>327</v>
-      </c>
-      <c r="P22" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>129</v>
-      </c>
-      <c r="R22" t="s">
-        <v>129</v>
-      </c>
-      <c r="S22" t="s">
-        <v>327</v>
-      </c>
-      <c r="X22" t="s">
-        <v>327</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>327</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>327</v>
-      </c>
-      <c r="AC22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AE22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AF22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AG22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AH22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AI22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AJ22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AK22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AL22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AN22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AO22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AP22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AQ22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AR22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AS22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AT22" t="s">
-        <v>327</v>
-      </c>
-      <c r="AU22" t="s">
-        <v>327</v>
-      </c>
-      <c r="AV22" t="s">
-        <v>327</v>
-      </c>
-      <c r="AW22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AY22" t="s">
-        <v>129</v>
-      </c>
-      <c r="AZ22" t="s">
-        <v>129</v>
-      </c>
-      <c r="BA22" t="s">
-        <v>129</v>
-      </c>
-      <c r="BB22" t="s">
-        <v>327</v>
-      </c>
-      <c r="BC22" t="s">
-        <v>129</v>
-      </c>
-      <c r="BE22" t="s">
-        <v>129</v>
-      </c>
-      <c r="BF22" t="s">
-        <v>129</v>
-      </c>
-      <c r="BG22" t="s">
-        <v>129</v>
-      </c>
-      <c r="BH22" t="s">
-        <v>129</v>
-      </c>
-      <c r="BI22" t="s">
-        <v>129</v>
-      </c>
-      <c r="BJ22" t="s">
-        <v>129</v>
-      </c>
-      <c r="BK22" t="s">
-        <v>327</v>
-      </c>
-      <c r="BL22" t="s">
-        <v>327</v>
-      </c>
-      <c r="BN22" t="s">
-        <v>327</v>
-      </c>
-      <c r="BP22" t="s">
-        <v>136</v>
-      </c>
-      <c r="BQ22" t="s">
-        <v>327</v>
-      </c>
-      <c r="BR22" t="s">
-        <v>327</v>
-      </c>
-      <c r="BS22" t="s">
-        <v>129</v>
-      </c>
-      <c r="BT22" t="s">
-        <v>129</v>
-      </c>
-      <c r="BU22" t="s">
-        <v>129</v>
-      </c>
-      <c r="BV22" t="s">
-        <v>129</v>
-      </c>
-      <c r="BW22" t="s">
-        <v>129</v>
-      </c>
-      <c r="CC22" t="s">
-        <v>327</v>
-      </c>
-      <c r="CE22" t="s">
-        <v>327</v>
-      </c>
       <c r="CG22" s="35" t="str">
         <f t="shared" ref="CG22:CL22" si="7">CONCATENATE(CG$1,"_","Ranged_Weaponry")</f>
         <v>Jarl_Ranged_Weaponry</v>
@@ -10509,165 +10847,6 @@
       </c>
     </row>
     <row r="23" spans="10:90" ht="15" x14ac:dyDescent="0.25">
-      <c r="J23" t="s">
-        <v>128</v>
-      </c>
-      <c r="K23" t="s">
-        <v>129</v>
-      </c>
-      <c r="L23" t="s">
-        <v>327</v>
-      </c>
-      <c r="M23" t="s">
-        <v>129</v>
-      </c>
-      <c r="N23" t="s">
-        <v>128</v>
-      </c>
-      <c r="P23" s="1"/>
-      <c r="Q23" t="s">
-        <v>327</v>
-      </c>
-      <c r="R23" t="s">
-        <v>327</v>
-      </c>
-      <c r="S23" t="s">
-        <v>128</v>
-      </c>
-      <c r="T23" s="29"/>
-      <c r="U23" s="29"/>
-      <c r="X23" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AD23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AE23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AF23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AG23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AH23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AI23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AJ23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AK23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AL23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AN23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AO23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AP23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AQ23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AR23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AS23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AU23" t="s">
-        <v>128</v>
-      </c>
-      <c r="AV23" t="s">
-        <v>128</v>
-      </c>
-      <c r="AW23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AY23" t="s">
-        <v>327</v>
-      </c>
-      <c r="AZ23" t="s">
-        <v>327</v>
-      </c>
-      <c r="BA23" t="s">
-        <v>327</v>
-      </c>
-      <c r="BB23" t="s">
-        <v>136</v>
-      </c>
-      <c r="BC23" t="s">
-        <v>327</v>
-      </c>
-      <c r="BE23" t="s">
-        <v>327</v>
-      </c>
-      <c r="BF23" t="s">
-        <v>327</v>
-      </c>
-      <c r="BG23" t="s">
-        <v>327</v>
-      </c>
-      <c r="BH23" t="s">
-        <v>327</v>
-      </c>
-      <c r="BI23" t="s">
-        <v>327</v>
-      </c>
-      <c r="BJ23" t="s">
-        <v>327</v>
-      </c>
-      <c r="BK23" t="s">
-        <v>128</v>
-      </c>
-      <c r="BL23" t="s">
-        <v>136</v>
-      </c>
-      <c r="BN23" t="s">
-        <v>136</v>
-      </c>
-      <c r="BP23" t="s">
-        <v>128</v>
-      </c>
-      <c r="BQ23" t="s">
-        <v>136</v>
-      </c>
-      <c r="BR23" t="s">
-        <v>136</v>
-      </c>
-      <c r="BS23" t="s">
-        <v>327</v>
-      </c>
-      <c r="BT23" t="s">
-        <v>327</v>
-      </c>
-      <c r="BU23" t="s">
-        <v>327</v>
-      </c>
-      <c r="BV23" t="s">
-        <v>327</v>
-      </c>
-      <c r="BW23" t="s">
-        <v>327</v>
-      </c>
       <c r="CG23" s="34" t="s">
         <v>147</v>
       </c>
@@ -10686,129 +10865,6 @@
       </c>
     </row>
     <row r="24" spans="10:90" ht="15" x14ac:dyDescent="0.25">
-      <c r="J24" t="s">
-        <v>129</v>
-      </c>
-      <c r="K24" t="s">
-        <v>327</v>
-      </c>
-      <c r="L24" t="s">
-        <v>136</v>
-      </c>
-      <c r="M24" t="s">
-        <v>327</v>
-      </c>
-      <c r="P24" s="1"/>
-      <c r="Q24" t="s">
-        <v>136</v>
-      </c>
-      <c r="R24" t="s">
-        <v>136</v>
-      </c>
-      <c r="T24" s="29"/>
-      <c r="U24" s="29"/>
-      <c r="AC24" t="s">
-        <v>136</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>136</v>
-      </c>
-      <c r="AE24" t="s">
-        <v>136</v>
-      </c>
-      <c r="AF24" t="s">
-        <v>136</v>
-      </c>
-      <c r="AG24" t="s">
-        <v>136</v>
-      </c>
-      <c r="AH24" t="s">
-        <v>136</v>
-      </c>
-      <c r="AI24" t="s">
-        <v>128</v>
-      </c>
-      <c r="AJ24" t="s">
-        <v>128</v>
-      </c>
-      <c r="AK24" t="s">
-        <v>128</v>
-      </c>
-      <c r="AL24" t="s">
-        <v>128</v>
-      </c>
-      <c r="AP24" t="s">
-        <v>136</v>
-      </c>
-      <c r="AQ24" t="s">
-        <v>136</v>
-      </c>
-      <c r="AR24" t="s">
-        <v>136</v>
-      </c>
-      <c r="AS24" t="s">
-        <v>136</v>
-      </c>
-      <c r="AW24" t="s">
-        <v>136</v>
-      </c>
-      <c r="AY24" t="s">
-        <v>136</v>
-      </c>
-      <c r="AZ24" t="s">
-        <v>136</v>
-      </c>
-      <c r="BA24" t="s">
-        <v>136</v>
-      </c>
-      <c r="BC24" t="s">
-        <v>136</v>
-      </c>
-      <c r="BE24" t="s">
-        <v>136</v>
-      </c>
-      <c r="BF24" t="s">
-        <v>136</v>
-      </c>
-      <c r="BG24" t="s">
-        <v>136</v>
-      </c>
-      <c r="BH24" t="s">
-        <v>136</v>
-      </c>
-      <c r="BI24" t="s">
-        <v>136</v>
-      </c>
-      <c r="BJ24" t="s">
-        <v>136</v>
-      </c>
-      <c r="BL24" t="s">
-        <v>128</v>
-      </c>
-      <c r="BN24" t="s">
-        <v>128</v>
-      </c>
-      <c r="BQ24" t="s">
-        <v>128</v>
-      </c>
-      <c r="BR24" t="s">
-        <v>128</v>
-      </c>
-      <c r="BS24" t="s">
-        <v>136</v>
-      </c>
-      <c r="BT24" t="s">
-        <v>136</v>
-      </c>
-      <c r="BU24" t="s">
-        <v>136</v>
-      </c>
-      <c r="BV24" t="s">
-        <v>136</v>
-      </c>
-      <c r="BW24" t="s">
-        <v>128</v>
-      </c>
       <c r="CG24" s="34"/>
       <c r="CH24" s="34"/>
       <c r="CI24" s="34" t="s">
@@ -10821,95 +10877,6 @@
       </c>
     </row>
     <row r="25" spans="10:90" ht="15" x14ac:dyDescent="0.25">
-      <c r="J25" t="s">
-        <v>136</v>
-      </c>
-      <c r="K25" s="1"/>
-      <c r="L25" t="s">
-        <v>128</v>
-      </c>
-      <c r="M25" t="s">
-        <v>136</v>
-      </c>
-      <c r="P25" s="1"/>
-      <c r="Q25" t="s">
-        <v>128</v>
-      </c>
-      <c r="R25" t="s">
-        <v>128</v>
-      </c>
-      <c r="S25" s="1"/>
-      <c r="T25" s="29"/>
-      <c r="U25" s="29"/>
-      <c r="AC25" t="s">
-        <v>128</v>
-      </c>
-      <c r="AD25" t="s">
-        <v>128</v>
-      </c>
-      <c r="AE25" t="s">
-        <v>128</v>
-      </c>
-      <c r="AF25" t="s">
-        <v>128</v>
-      </c>
-      <c r="AG25" t="s">
-        <v>128</v>
-      </c>
-      <c r="AH25" t="s">
-        <v>128</v>
-      </c>
-      <c r="AP25" t="s">
-        <v>128</v>
-      </c>
-      <c r="AQ25" t="s">
-        <v>128</v>
-      </c>
-      <c r="AR25" t="s">
-        <v>128</v>
-      </c>
-      <c r="AS25" t="s">
-        <v>128</v>
-      </c>
-      <c r="AW25" t="s">
-        <v>128</v>
-      </c>
-      <c r="AY25" t="s">
-        <v>128</v>
-      </c>
-      <c r="AZ25" t="s">
-        <v>128</v>
-      </c>
-      <c r="BE25" t="s">
-        <v>128</v>
-      </c>
-      <c r="BF25" t="s">
-        <v>128</v>
-      </c>
-      <c r="BG25" t="s">
-        <v>128</v>
-      </c>
-      <c r="BH25" t="s">
-        <v>128</v>
-      </c>
-      <c r="BI25" t="s">
-        <v>128</v>
-      </c>
-      <c r="BJ25" t="s">
-        <v>128</v>
-      </c>
-      <c r="BS25" t="s">
-        <v>128</v>
-      </c>
-      <c r="BT25" t="s">
-        <v>128</v>
-      </c>
-      <c r="BU25" t="s">
-        <v>128</v>
-      </c>
-      <c r="BV25" t="s">
-        <v>128</v>
-      </c>
       <c r="CG25" s="34"/>
       <c r="CH25" s="34"/>
       <c r="CI25" s="34"/>
@@ -10918,20 +10885,6 @@
       <c r="CL25" s="34"/>
     </row>
     <row r="26" spans="10:90" ht="15" x14ac:dyDescent="0.25">
-      <c r="J26" t="s">
-        <v>327</v>
-      </c>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" t="s">
-        <v>128</v>
-      </c>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="29"/>
-      <c r="U26" s="29"/>
       <c r="CG26" s="34"/>
       <c r="CH26" s="34"/>
       <c r="CI26" s="34"/>
@@ -10940,15 +10893,6 @@
       <c r="CL26" s="34"/>
     </row>
     <row r="27" spans="10:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="29"/>
-      <c r="U27" s="29"/>
       <c r="CG27" s="35" t="str">
         <f t="shared" ref="CG27:CL27" si="8">CONCATENATE(CG$1,"_","Armour")</f>
         <v>Jarl_Armour</v>
@@ -13501,7 +13445,7 @@
         <v>Empire_State_Troop_Mounts</v>
       </c>
       <c r="K60" s="42" t="str">
-        <f t="shared" ref="K60:CE60" si="21">CONCATENATE(K$1,"_","Mounts")</f>
+        <f t="shared" ref="K60:CF60" si="21">CONCATENATE(K$1,"_","Mounts")</f>
         <v>Empire_State_Troop_Skirmisher_Mounts</v>
       </c>
       <c r="L60" s="42" t="str">
@@ -13792,7 +13736,7 @@
         <f t="shared" si="21"/>
         <v>Ashiguru_Mounts</v>
       </c>
-      <c r="CG60" s="42" t="str">
+      <c r="CF60" s="42" t="str">
         <f>CONCATENATE(CF$1,"_","Mounts")</f>
         <v>Nipponese_Leves_Mounts</v>
       </c>
@@ -13944,7 +13888,7 @@
     <row r="64" spans="1:90" x14ac:dyDescent="0.2">
       <c r="L64" s="1"/>
     </row>
-    <row r="65" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="42"/>
       <c r="B65" s="42"/>
       <c r="C65" s="42"/>
@@ -14223,7 +14167,7 @@
         <v>Dragonblade_Armour</v>
       </c>
       <c r="BY65" s="42" t="str">
-        <f t="shared" ref="BY65:CE65" si="23">CONCATENATE(BY$1,"_","Armour")</f>
+        <f t="shared" ref="BY65:CF65" si="23">CONCATENATE(BY$1,"_","Armour")</f>
         <v>Imperial_Guard_Armour</v>
       </c>
       <c r="BZ65" s="42" t="str">
@@ -14250,12 +14194,12 @@
         <f t="shared" si="23"/>
         <v>Ashiguru_Armour</v>
       </c>
-      <c r="CG65" s="42" t="str">
+      <c r="CF65" s="42" t="str">
         <f>CONCATENATE(CF$1,"_","Armour")</f>
         <v>Nipponese_Leves_Armour</v>
       </c>
     </row>
-    <row r="66" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:84" x14ac:dyDescent="0.2">
       <c r="J66" t="s">
         <v>341</v>
       </c>
@@ -14427,11 +14371,11 @@
       <c r="CE66" t="s">
         <v>233</v>
       </c>
-      <c r="CG66" t="s">
+      <c r="CF66" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="67" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:84" x14ac:dyDescent="0.2">
       <c r="J67" t="s">
         <v>233</v>
       </c>
@@ -14550,7 +14494,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="68" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:84" x14ac:dyDescent="0.2">
       <c r="J68" t="s">
         <v>346</v>
       </c>
@@ -14663,7 +14607,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="69" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:84" x14ac:dyDescent="0.2">
       <c r="M69" t="s">
         <v>346</v>
       </c>
@@ -14746,7 +14690,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="70" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:84" x14ac:dyDescent="0.2">
       <c r="M70" t="s">
         <v>330</v>
       </c>
@@ -14796,7 +14740,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="71" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:84" x14ac:dyDescent="0.2">
       <c r="M71" t="s">
         <v>348</v>
       </c>
@@ -14804,12 +14748,12 @@
         <v>330</v>
       </c>
     </row>
-    <row r="72" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:84" x14ac:dyDescent="0.2">
       <c r="BC72" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="74" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="42"/>
       <c r="B74" s="42"/>
       <c r="C74" s="42"/>
@@ -15115,12 +15059,12 @@
         <f>CONCATENATE(CE$1,"_","Helmet")</f>
         <v>Ashiguru_Helmet</v>
       </c>
-      <c r="CG74" s="42" t="str">
+      <c r="CF74" s="42" t="str">
         <f>CONCATENATE(CF$1,"_","Helmet")</f>
         <v>Nipponese_Leves_Helmet</v>
       </c>
     </row>
-    <row r="75" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:84" x14ac:dyDescent="0.2">
       <c r="J75" t="s">
         <v>238</v>
       </c>
@@ -15280,11 +15224,11 @@
       <c r="CE75" t="s">
         <v>238</v>
       </c>
-      <c r="CG75" t="s">
+      <c r="CF75" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="78" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J78" s="42" t="str">
         <f>CONCATENATE(J$1,"_","Mounts")</f>
         <v>Empire_State_Troop_Mounts</v>
@@ -15546,7 +15490,7 @@
         <v>Imperial_Infantry_Mounts</v>
       </c>
       <c r="BW78" s="42" t="str">
-        <f t="shared" ref="BW78:CE78" si="27">CONCATENATE(BW$1,"_","Mounts")</f>
+        <f t="shared" ref="BW78:CF78" si="27">CONCATENATE(BW$1,"_","Mounts")</f>
         <v>Levy-Infantry_Mounts</v>
       </c>
       <c r="BX78" s="42" t="str">
@@ -15581,12 +15525,12 @@
         <f t="shared" si="27"/>
         <v>Ashiguru_Mounts</v>
       </c>
-      <c r="CG78" s="42" t="str">
+      <c r="CF78" s="42" t="str">
         <f>CONCATENATE(CF$1,"_","Mounts")</f>
         <v>Nipponese_Leves_Mounts</v>
       </c>
     </row>
-    <row r="79" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:84" x14ac:dyDescent="0.2">
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
       <c r="L79" s="1" t="s">
@@ -15680,7 +15624,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="80" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:84" x14ac:dyDescent="0.2">
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
@@ -20595,7 +20539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AMC49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>

</xml_diff>